<commit_message>
Goal --> Additional topics
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-expressed-by.xlsx
+++ b/output/StructureDefinition-expressed-by.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="67">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2023-07-17T09:56:27+02:00</t>
+    <t>2023-07-17T16:21:50+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -209,6 +209,10 @@
   </si>
   <si>
     <t>Extension.value[x]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference(Patient|Practitioner|RelatedPerson)
+</t>
   </si>
   <si>
     <t>Value of extension</t>
@@ -538,7 +542,7 @@
     <col min="8" max="8" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="1.04296875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="9.734375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="41.1875" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1008,13 +1012,13 @@
         <v>36</v>
       </c>
       <c r="K5" t="s" s="2">
-        <v>43</v>
+        <v>63</v>
       </c>
       <c r="L5" t="s" s="2">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="M5" t="s" s="2">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
@@ -1077,7 +1081,7 @@
         <v>36</v>
       </c>
       <c r="AJ5" t="s" s="2">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AK5" t="s" s="2">
         <v>61</v>

</xml_diff>